<commit_message>
doc: change excel sheet name
</commit_message>
<xml_diff>
--- a/twcore/excel-template-with10-sample-data/Location.xlsx
+++ b/twcore/excel-template-with10-sample-data/Location.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GoogleDrive\My Data\School Data\國北護\【Lab Projects】\RedpandaV2\TW_Core_IG_CSV_format\各FHIR Resource共編\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\FHIR-Universal-Conversion-Kit\twcore\excel-template-with10-sample-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BCC9DF-F325-4B4F-8125-BC7C1D14F74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B58F67-7FFD-4B7C-904A-67BB1284702F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="10125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Organization" sheetId="1" r:id="rId1"/>
+    <sheet name="Location" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -654,30 +654,30 @@
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="44" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="54.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,7 +748,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -807,7 +807,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -866,7 +866,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -925,7 +925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -984,7 +984,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>

</xml_diff>